<commit_message>
03/19/23: more training runs
</commit_message>
<xml_diff>
--- a/experiments_training_characteristics.xlsx
+++ b/experiments_training_characteristics.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ad2we\Desktop\2022_2023_Stanford\winqtr_2023\cs224n_dfp\minbert-default-final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59D15F3-8F72-41F5-9629-21300D618F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E979BE-4D52-4651-A4D4-893B419C4DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5295" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{D62B41D3-5484-473B-8634-D66484C1623D}"/>
+    <workbookView xWindow="-28920" yWindow="5295" windowWidth="29040" windowHeight="16440" xr2:uid="{D62B41D3-5484-473B-8634-D66484C1623D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
   <si>
     <r>
       <t xml:space="preserve">MODELS USING </t>
@@ -142,9 +141,6 @@
     <t>ABSOLUTE AND RELATIVE SCORES USING DIFFERENT HARD PARAMETER SHARING REGIMES AND FIXED LEARNING RATES</t>
   </si>
   <si>
-    <t>ABSOLUTE AND RELATIVE SCORES USING FREELY VARYING PARAMETER SHARING REGIMES AND FREELY VARYING LEARNING RATES</t>
-  </si>
-  <si>
     <t>EXPR. 1</t>
   </si>
   <si>
@@ -190,25 +186,13 @@
     <t>PreTr</t>
   </si>
   <si>
-    <t xml:space="preserve">regime </t>
-  </si>
-  <si>
-    <t>lr</t>
-  </si>
-  <si>
-    <t>iss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">score </t>
-  </si>
-  <si>
-    <t>para</t>
-  </si>
-  <si>
-    <t>senti</t>
-  </si>
-  <si>
-    <t>sts</t>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>ABSOLUTE AND RELATIVE SCORES USING FREELY VARYING PARAMETER SHARING REGIMES, TASK-SPECIFIC LOSS WEIGHTS, AND LEARNING RATES</t>
+  </si>
+  <si>
+    <t>Non-uniform task-specific loss - [0.4, 0.2, 0.4].</t>
   </si>
 </sst>
 </file>
@@ -218,7 +202,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,14 +234,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFAE81FF"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +281,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -511,16 +495,39 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,11 +848,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15CB41C-6E4C-4CF1-BCAA-DFE6D6233FB9}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +872,7 @@
     <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -889,7 +896,7 @@
       <c r="O1" s="29"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R1" s="13"/>
     </row>
@@ -917,7 +924,7 @@
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>16</v>
@@ -935,34 +942,34 @@
         <v>17</v>
       </c>
       <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="P3" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="Q3" s="38"/>
       <c r="R3" s="13"/>
@@ -1019,7 +1026,7 @@
       <c r="Q4" s="38"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="40" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4"/>
@@ -1117,7 +1124,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="40" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4"/>
@@ -1134,7 +1141,7 @@
         <v>1E-3</v>
       </c>
       <c r="G7" s="23">
-        <v>8</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="H7" s="14">
         <v>6</v>
@@ -1156,17 +1163,17 @@
       </c>
       <c r="N7" s="23">
         <f>G7 * $L$4/L7 * $M$4/M7</f>
-        <v>7.6738691804289774</v>
+        <v>0.32805790746333874</v>
       </c>
       <c r="O7" s="13">
         <f t="shared" si="1"/>
-        <v>0.95923364755362217</v>
+        <v>0.95923364755362195</v>
       </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="38"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4"/>
@@ -1212,7 +1219,7 @@
         <v>1.0555495541876196</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="38"/>
     </row>
@@ -1266,7 +1273,7 @@
       <c r="Q9" s="38"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="4"/>
@@ -1361,7 +1368,7 @@
         <v>1.040182223967647</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="38"/>
     </row>
@@ -1388,7 +1395,7 @@
     </row>
     <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>16</v>
@@ -1406,34 +1413,34 @@
         <v>17</v>
       </c>
       <c r="G13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="P13" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="P13" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="Q13" s="38"/>
     </row>
@@ -1587,7 +1594,7 @@
       <c r="Q16" s="38"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="40" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="4"/>
@@ -1606,22 +1613,22 @@
       <c r="G17" s="23">
         <v>0.49399999999999999</v>
       </c>
-      <c r="H17" s="41">
+      <c r="H17" s="42">
         <v>5</v>
       </c>
-      <c r="I17" s="42">
+      <c r="I17" s="43">
         <v>0.627</v>
       </c>
-      <c r="J17" s="42">
+      <c r="J17" s="43">
         <v>0.503</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K17" s="43">
         <v>0.35299999999999998</v>
       </c>
-      <c r="L17" s="43">
+      <c r="L17" s="44">
         <v>5725.13</v>
       </c>
-      <c r="M17" s="41">
+      <c r="M17" s="42">
         <v>1338657</v>
       </c>
       <c r="N17" s="23">
@@ -1636,7 +1643,7 @@
       <c r="Q17" s="38"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="60" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="4"/>
@@ -1685,7 +1692,7 @@
       <c r="Q18" s="38"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="4"/>
@@ -1734,7 +1741,7 @@
       <c r="Q19" s="38"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="4"/>
@@ -1771,7 +1778,7 @@
       <c r="M20">
         <v>1324811</v>
       </c>
-      <c r="N20" s="40">
+      <c r="N20" s="41">
         <f t="shared" si="2"/>
         <v>0.58656585956354645</v>
       </c>
@@ -1834,7 +1841,7 @@
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B23" s="35"/>
       <c r="C23" s="35"/>
@@ -1856,131 +1863,263 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="I24" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="N24" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="10" t="s">
+      <c r="O24" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="P24" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L24" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M24" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="N24" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O24" s="10" t="s">
+      <c r="Q24" s="38"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="P24" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q24" s="38"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25">
+      <c r="C25" s="16">
         <v>10</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="16">
         <v>1000</v>
       </c>
-      <c r="E25">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="E25" s="16">
+        <v>8</v>
+      </c>
+      <c r="F25" s="17">
         <v>8.5648770269280502E-6</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="16">
         <v>0.39200000000000002</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="16">
         <v>9</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="16">
         <v>0.61799999999999999</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="16">
         <v>0.38600000000000001</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="16">
         <v>0.17299999999999999</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="16">
         <v>3210.24</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="16">
         <v>469359</v>
       </c>
-      <c r="N25" s="13">
+      <c r="N25" s="18">
         <f>G25 * $L$4/L25 * $M$4/M25</f>
         <v>0.4122532064130161</v>
       </c>
-      <c r="O25" s="13">
+      <c r="O25" s="18">
         <f>N25/G25</f>
         <v>1.0516663428903472</v>
       </c>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="38"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6">
+      <c r="P25" s="21"/>
+      <c r="Q25" s="46"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="51">
         <v>10</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="51">
         <v>1000</v>
       </c>
-      <c r="E26" s="6">
-        <v>8</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="39"/>
+      <c r="E26" s="51">
+        <v>8</v>
+      </c>
+      <c r="F26" s="52">
+        <v>8.5648770269280502E-6</v>
+      </c>
+      <c r="G26" s="57">
+        <v>0.313</v>
+      </c>
+      <c r="H26" s="57">
+        <v>9</v>
+      </c>
+      <c r="I26" s="51">
+        <v>0.375</v>
+      </c>
+      <c r="J26" s="51">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="K26" s="51">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="L26" s="57">
+        <v>3469.92</v>
+      </c>
+      <c r="M26" s="57">
+        <v>469359</v>
+      </c>
+      <c r="N26" s="53">
+        <f>G26 * $L$4/L26 * $M$4/M26</f>
+        <v>0.30453720139596774</v>
+      </c>
+      <c r="O26" s="53">
+        <f>N26/G26</f>
+        <v>0.97296230477944967</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q26" s="46"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="51">
+        <v>10</v>
+      </c>
+      <c r="D27" s="51">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="51">
+        <v>8</v>
+      </c>
+      <c r="F27" s="52">
+        <v>8.5658800000000007E-6</v>
+      </c>
+      <c r="G27" s="59">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="H27" s="57">
+        <v>6</v>
+      </c>
+      <c r="I27" s="57">
+        <v>0.375</v>
+      </c>
+      <c r="J27" s="57">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="K27" s="57">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="L27" s="57">
+        <v>5434.68</v>
+      </c>
+      <c r="M27" s="57">
+        <v>1338657</v>
+      </c>
+      <c r="N27" s="53">
+        <f>G27 * $L$14/L27 * $M$14/M27</f>
+        <v>0.47106595737019064</v>
+      </c>
+      <c r="O27" s="53">
+        <f>N27/G27</f>
+        <v>1.1865641243581628</v>
+      </c>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="46"/>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="6">
+        <v>10</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E28" s="6">
+        <v>8</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="H28" s="58">
+        <v>5</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="K28" s="6">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="L28" s="6">
+        <v>5340.03</v>
+      </c>
+      <c r="M28" s="6">
+        <v>1324811</v>
+      </c>
+      <c r="N28" s="22">
+        <f>G28 * $L$14/L28 * $M$14/M28</f>
+        <v>0.60156671854229349</v>
+      </c>
+      <c r="O28" s="22">
+        <f>N28/G28</f>
+        <v>1.2202164676314269</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q28" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1988,94 +2127,8 @@
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="A12:P12"/>
     <mergeCell ref="A23:P23"/>
-    <mergeCell ref="Q23:Q26"/>
     <mergeCell ref="Q1:Q21"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E644D60-9D41-4DA5-81E3-0E2E9E73951A}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="44">
-        <v>5.6883799999999999E-5</v>
-      </c>
-      <c r="C2">
-        <v>0.37494</v>
-      </c>
-      <c r="D2">
-        <v>0.375</v>
-      </c>
-      <c r="E2">
-        <v>0.439</v>
-      </c>
-      <c r="F2">
-        <v>0.27900000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="44">
-        <v>2.5494699999999999E-6</v>
-      </c>
-      <c r="C3">
-        <v>0.33458300000000002</v>
-      </c>
-      <c r="D3">
-        <v>0.375</v>
-      </c>
-      <c r="E3">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="F3">
-        <v>0.27800000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44">
-        <v>4.5866499999999998E-7</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="Q23:Q28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
03/21/22: final code push!
</commit_message>
<xml_diff>
--- a/experiments_training_characteristics.xlsx
+++ b/experiments_training_characteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ad2we\Desktop\2022_2023_Stanford\winqtr_2023\cs224n_dfp\minbert-default-final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E979BE-4D52-4651-A4D4-893B419C4DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4627E07C-854E-4B42-9DCC-E82E053B16B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5295" windowWidth="29040" windowHeight="16440" xr2:uid="{D62B41D3-5484-473B-8634-D66484C1623D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28020" windowHeight="16440" xr2:uid="{D62B41D3-5484-473B-8634-D66484C1623D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
   <si>
     <r>
       <t xml:space="preserve">MODELS USING </t>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>Non-uniform task-specific loss - [0.4, 0.2, 0.4].</t>
+  </si>
+  <si>
+    <t>ABSOLUTE AND RELATIVE SCORES USING SUBSET PARAMETER SHARING</t>
+  </si>
+  <si>
+    <t>[0] I-S-S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*using new STS logit comp. </t>
+  </si>
+  <si>
+    <t>*using old STS logit comp.</t>
   </si>
 </sst>
 </file>
@@ -420,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -459,6 +471,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,57 +528,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,11 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15CB41C-6E4C-4CF1-BCAA-DFE6D6233FB9}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K28" sqref="K28"/>
+      <selection pane="topRight" activeCell="A32" sqref="A32:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,49 +880,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="37" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="41" t="s">
         <v>19</v>
       </c>
       <c r="R1" s="13"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="38"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="42"/>
       <c r="R2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -971,7 +974,7 @@
       <c r="P3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="38"/>
+      <c r="Q3" s="42"/>
       <c r="R3" s="13"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1023,10 +1026,10 @@
         <v>1</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="38"/>
+      <c r="Q4" s="42"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4"/>
@@ -1072,7 +1075,7 @@
         <v>1.0085686138400722</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="38"/>
+      <c r="Q5" s="42"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1121,10 +1124,10 @@
         <v>1.027777608227896</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="38"/>
+      <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4"/>
@@ -1170,10 +1173,10 @@
         <v>0.95923364755362195</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="38"/>
+      <c r="Q7" s="42"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4"/>
@@ -1221,7 +1224,7 @@
       <c r="P8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="38"/>
+      <c r="Q8" s="42"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1270,10 +1273,10 @@
         <v>0.92982237527239953</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="38"/>
+      <c r="Q9" s="42"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="4"/>
@@ -1319,7 +1322,7 @@
         <v>0.99590891972504436</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="38"/>
+      <c r="Q10" s="42"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1370,28 +1373,28 @@
       <c r="P11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q11" s="38"/>
+      <c r="Q11" s="42"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="38"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="42"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
@@ -1442,7 +1445,7 @@
       <c r="P13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="Q13" s="38"/>
+      <c r="Q13" s="42"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1493,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="P14" s="21"/>
-      <c r="Q14" s="38"/>
+      <c r="Q14" s="42"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1542,7 +1545,7 @@
         <v>1.1259360949565975</v>
       </c>
       <c r="P15" s="3"/>
-      <c r="Q15" s="38"/>
+      <c r="Q15" s="42"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1591,10 +1594,10 @@
         <v>1.2561792763936535</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="38"/>
+      <c r="Q16" s="42"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="4"/>
@@ -1613,22 +1616,22 @@
       <c r="G17" s="23">
         <v>0.49399999999999999</v>
       </c>
-      <c r="H17" s="42">
+      <c r="H17">
         <v>5</v>
       </c>
-      <c r="I17" s="43">
+      <c r="I17" s="13">
         <v>0.627</v>
       </c>
-      <c r="J17" s="43">
+      <c r="J17" s="13">
         <v>0.503</v>
       </c>
-      <c r="K17" s="43">
+      <c r="K17" s="13">
         <v>0.35299999999999998</v>
       </c>
-      <c r="L17" s="44">
+      <c r="L17" s="12">
         <v>5725.13</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M17">
         <v>1338657</v>
       </c>
       <c r="N17" s="23">
@@ -1640,10 +1643,10 @@
         <v>1.1263667926085204</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="38"/>
+      <c r="Q17" s="42"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="4"/>
@@ -1689,10 +1692,10 @@
         <v>1.1518602039703245</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="38"/>
+      <c r="Q18" s="42"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="4"/>
@@ -1738,10 +1741,10 @@
         <v>1.2368818513852957</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="38"/>
+      <c r="Q19" s="42"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="4"/>
@@ -1778,7 +1781,7 @@
       <c r="M20">
         <v>1324811</v>
       </c>
-      <c r="N20" s="41">
+      <c r="N20" s="29">
         <f t="shared" si="2"/>
         <v>0.58656585956354645</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>1.1970731827827479</v>
       </c>
       <c r="P20" s="3"/>
-      <c r="Q20" s="38"/>
+      <c r="Q20" s="42"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
@@ -1836,85 +1839,85 @@
         <v>1.1655062683566157</v>
       </c>
       <c r="P21" s="8"/>
-      <c r="Q21" s="39"/>
+      <c r="Q21" s="51"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="37">
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="41">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="49" t="s">
+      <c r="F24" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="49" t="s">
+      <c r="G24" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="49" t="s">
+      <c r="H24" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="49" t="s">
+      <c r="I24" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="49" t="s">
+      <c r="J24" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="K24" s="49" t="s">
+      <c r="K24" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="L24" s="49" t="s">
+      <c r="L24" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="M24" s="49" t="s">
+      <c r="M24" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="N24" s="49" t="s">
+      <c r="N24" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="O24" s="49" t="s">
+      <c r="O24" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="P24" s="50" t="s">
+      <c r="P24" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Q24" s="38"/>
+      <c r="Q24" s="42"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="15" t="s">
@@ -1962,117 +1965,117 @@
         <v>1.0516663428903472</v>
       </c>
       <c r="P25" s="21"/>
-      <c r="Q25" s="46"/>
+      <c r="Q25" s="43"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="35" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26">
         <v>10</v>
       </c>
-      <c r="D26" s="51">
+      <c r="D26">
         <v>1000</v>
       </c>
-      <c r="E26" s="51">
-        <v>8</v>
-      </c>
-      <c r="F26" s="52">
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26" s="2">
         <v>8.5648770269280502E-6</v>
       </c>
-      <c r="G26" s="57">
+      <c r="G26">
         <v>0.313</v>
       </c>
-      <c r="H26" s="57">
+      <c r="H26">
         <v>9</v>
       </c>
-      <c r="I26" s="51">
+      <c r="I26">
         <v>0.375</v>
       </c>
-      <c r="J26" s="51">
+      <c r="J26">
         <v>0.36399999999999999</v>
       </c>
-      <c r="K26" s="51">
+      <c r="K26">
         <v>0.19900000000000001</v>
       </c>
-      <c r="L26" s="57">
+      <c r="L26">
         <v>3469.92</v>
       </c>
-      <c r="M26" s="57">
+      <c r="M26">
         <v>469359</v>
       </c>
-      <c r="N26" s="53">
+      <c r="N26" s="13">
         <f>G26 * $L$4/L26 * $M$4/M26</f>
         <v>0.30453720139596774</v>
       </c>
-      <c r="O26" s="53">
+      <c r="O26" s="13">
         <f>N26/G26</f>
         <v>0.97296230477944967</v>
       </c>
       <c r="P26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Q26" s="46"/>
+      <c r="Q26" s="43"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="51">
+      <c r="C27">
         <v>10</v>
       </c>
-      <c r="D27" s="51">
+      <c r="D27">
         <v>1000</v>
       </c>
-      <c r="E27" s="51">
-        <v>8</v>
-      </c>
-      <c r="F27" s="52">
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27" s="2">
         <v>8.5658800000000007E-6</v>
       </c>
-      <c r="G27" s="59">
+      <c r="G27" s="13">
         <v>0.39700000000000002</v>
       </c>
-      <c r="H27" s="57">
+      <c r="H27">
         <v>6</v>
       </c>
-      <c r="I27" s="57">
+      <c r="I27">
         <v>0.375</v>
       </c>
-      <c r="J27" s="57">
+      <c r="J27">
         <v>0.49099999999999999</v>
       </c>
-      <c r="K27" s="57">
+      <c r="K27">
         <v>0.32500000000000001</v>
       </c>
-      <c r="L27" s="57">
+      <c r="L27">
         <v>5434.68</v>
       </c>
-      <c r="M27" s="57">
+      <c r="M27">
         <v>1338657</v>
       </c>
-      <c r="N27" s="53">
+      <c r="N27" s="13">
         <f>G27 * $L$14/L27 * $M$14/M27</f>
         <v>0.47106595737019064</v>
       </c>
-      <c r="O27" s="53">
+      <c r="O27" s="13">
         <f>N27/G27</f>
         <v>1.1865641243581628</v>
       </c>
       <c r="P27" s="3"/>
-      <c r="Q27" s="46"/>
+      <c r="Q27" s="43"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="6">
@@ -2090,7 +2093,7 @@
       <c r="G28" s="6">
         <v>0.49299999999999999</v>
       </c>
-      <c r="H28" s="58">
+      <c r="H28" s="6">
         <v>5</v>
       </c>
       <c r="I28" s="6">
@@ -2119,10 +2122,193 @@
       <c r="P28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q28" s="47"/>
+      <c r="Q28" s="44"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="M31" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="O31" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="P31" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q31" s="42"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="16">
+        <v>10</v>
+      </c>
+      <c r="D32" s="16">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="16">
+        <v>8</v>
+      </c>
+      <c r="F32" s="17">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G32" s="16">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="H32" s="16">
+        <v>5</v>
+      </c>
+      <c r="I32" s="16">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="J32" s="16">
+        <v>0.49</v>
+      </c>
+      <c r="K32" s="16">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="L32" s="16">
+        <v>6614.49</v>
+      </c>
+      <c r="M32" s="16">
+        <v>1338657</v>
+      </c>
+      <c r="N32" s="18">
+        <f>G32 * $L$14/L32 * $M$14/M32</f>
+        <v>0.55082960563584682</v>
+      </c>
+      <c r="O32" s="18">
+        <f>N32/G32</f>
+        <v>0.97491965599264929</v>
+      </c>
+      <c r="P32" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q32" s="43"/>
+    </row>
+    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="6">
+        <v>10</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E33" s="6">
+        <v>8</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H33" s="6">
+        <v>7</v>
+      </c>
+      <c r="I33" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="J33" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="K33" s="6">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="L33" s="6">
+        <v>5612.81</v>
+      </c>
+      <c r="M33" s="6">
+        <v>1338657</v>
+      </c>
+      <c r="N33" s="22">
+        <f>G33 * $L$14/L33 * $M$14/M33</f>
+        <v>0.55836876881068009</v>
+      </c>
+      <c r="O33" s="22">
+        <f>N33/G33</f>
+        <v>1.1489069317092184</v>
+      </c>
+      <c r="P33" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q33" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A30:P30"/>
+    <mergeCell ref="Q30:Q33"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="A12:P12"/>

</xml_diff>